<commit_message>
feat: better date value handling and tests support added
</commit_message>
<xml_diff>
--- a/test/assets/rules.xlsx
+++ b/test/assets/rules.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vlad/Workspace/FireBlink/rulex/test/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E27C42D-2B29-E645-9016-00D3A86B78F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFBE20D-70F6-474E-839B-68B3510C248A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="2620" windowWidth="27240" windowHeight="16440" xr2:uid="{0B955657-EF69-9248-BFB1-36373A7557EB}"/>
+    <workbookView xWindow="6160" yWindow="1240" windowWidth="27240" windowHeight="16440" activeTab="4" xr2:uid="{0B955657-EF69-9248-BFB1-36373A7557EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Context" sheetId="1" r:id="rId1"/>
-    <sheet name="Step 1 - Condition + Action" sheetId="2" r:id="rId2"/>
-    <sheet name="Step 2 - If + Set" sheetId="3" r:id="rId3"/>
-    <sheet name="Step 3 - Break" sheetId="4" r:id="rId4"/>
-    <sheet name="Step 4 - Void" sheetId="5" r:id="rId5"/>
+    <sheet name="Tests" sheetId="6" r:id="rId2"/>
+    <sheet name="Step 1 - Condition + Action" sheetId="2" r:id="rId3"/>
+    <sheet name="Step 2 - If + Set" sheetId="3" r:id="rId4"/>
+    <sheet name="Step 3 - Break" sheetId="4" r:id="rId5"/>
+    <sheet name="Step 4 - Void" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -157,6 +158,60 @@
   </si>
   <si>
     <t>Set context.step4</t>
+  </si>
+  <si>
+    <t>Set fact.boolValue</t>
+  </si>
+  <si>
+    <t>Set fact.intValue</t>
+  </si>
+  <si>
+    <t>Set fact.floatValue</t>
+  </si>
+  <si>
+    <t>Set fact.dateValue</t>
+  </si>
+  <si>
+    <t>Set fact.strValue</t>
+  </si>
+  <si>
+    <t>Set fact.break</t>
+  </si>
+  <si>
+    <t>string with spaces</t>
+  </si>
+  <si>
+    <t>Expect context["Simple Condition"]</t>
+  </si>
+  <si>
+    <t>Step 1 - Condition + Action</t>
+  </si>
+  <si>
+    <t>Expect context["Complex Condition"]</t>
+  </si>
+  <si>
+    <t>Expect context["Empty Condition"]</t>
+  </si>
+  <si>
+    <t>Expect context["String Condition"]</t>
+  </si>
+  <si>
+    <t>Expect context.Math</t>
+  </si>
+  <si>
+    <t>Set context.step2date</t>
+  </si>
+  <si>
+    <t>If context.initDateValue</t>
+  </si>
+  <si>
+    <t>Expect fact.break</t>
+  </si>
+  <si>
+    <t>Expect result.step1</t>
+  </si>
+  <si>
+    <t>Set result.step1</t>
   </si>
 </sst>
 </file>
@@ -203,7 +258,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,6 +289,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -247,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -258,6 +325,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DCA8C4C-64FA-DC43-BD12-6D78521EDD2A}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -637,11 +706,129 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D85D4E-B609-BA4D-A7F3-29129ADE1C24}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="18.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>5.5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44927</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA23193F-2081-EF4F-B2C7-982DC8DDF8B9}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -649,9 +836,10 @@
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -664,8 +852,11 @@
       <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -675,8 +866,11 @@
       <c r="C2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -686,16 +880,22 @@
       <c r="C3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -705,8 +905,11 @@
       <c r="C5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -715,6 +918,9 @@
       </c>
       <c r="C6" t="s">
         <v>34</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -722,12 +928,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D441B4-1056-A04E-8DBE-9BFDDA9B96D4}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -735,10 +941,12 @@
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -748,14 +956,20 @@
       <c r="C1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>36</v>
+      <c r="D1" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -765,11 +979,17 @@
       <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D2" s="1">
+        <v>44774</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>44562</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -779,19 +999,31 @@
       <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="1">
+        <v>44774</v>
+      </c>
+      <c r="E3" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G3" s="1">
+        <v>44563</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
+        <v>44774</v>
+      </c>
+      <c r="E4">
         <v>3</v>
+      </c>
+      <c r="G4" s="1">
+        <v>44564</v>
       </c>
     </row>
   </sheetData>
@@ -799,12 +1031,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F02A80BA-6F4C-824B-A578-DF6E4A06F5CC}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -865,17 +1097,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB756B9-053B-3A49-ADCA-1E4932B679E4}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="H23" activeCellId="1" sqref="D11 H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat: add single cli to run tests over the provided rules file
</commit_message>
<xml_diff>
--- a/test/assets/rules.xlsx
+++ b/test/assets/rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vlad/Workspace/FireBlink/rulex/test/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFBE20D-70F6-474E-839B-68B3510C248A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40295FD-C7E8-C74B-90C0-76F05A082789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6160" yWindow="1240" windowWidth="27240" windowHeight="16440" activeTab="4" xr2:uid="{0B955657-EF69-9248-BFB1-36373A7557EB}"/>
+    <workbookView xWindow="6160" yWindow="1240" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{0B955657-EF69-9248-BFB1-36373A7557EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Context" sheetId="1" r:id="rId1"/>
@@ -709,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D85D4E-B609-BA4D-A7F3-29129ADE1C24}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1035,7 +1035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F02A80BA-6F4C-824B-A578-DF6E4A06F5CC}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: add in and out conditions
</commit_message>
<xml_diff>
--- a/test/assets/rules.xlsx
+++ b/test/assets/rules.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vlad/Workspace/FireBlink/rulex/test/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40295FD-C7E8-C74B-90C0-76F05A082789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098A4FB9-3376-734C-BA62-3FC6F5139BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6160" yWindow="1240" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{0B955657-EF69-9248-BFB1-36373A7557EB}"/>
+    <workbookView xWindow="6160" yWindow="1240" windowWidth="27240" windowHeight="16440" activeTab="4" xr2:uid="{0B955657-EF69-9248-BFB1-36373A7557EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Context" sheetId="1" r:id="rId1"/>
     <sheet name="Tests" sheetId="6" r:id="rId2"/>
     <sheet name="Step 1 - Condition + Action" sheetId="2" r:id="rId3"/>
     <sheet name="Step 2 - If + Set" sheetId="3" r:id="rId4"/>
-    <sheet name="Step 3 - Break" sheetId="4" r:id="rId5"/>
-    <sheet name="Step 4 - Void" sheetId="5" r:id="rId6"/>
+    <sheet name="Step 3 - In + Out" sheetId="7" r:id="rId5"/>
+    <sheet name="Step 4 - Break" sheetId="4" r:id="rId6"/>
+    <sheet name="Step 5 - Void" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -157,9 +158,6 @@
     <t>If fact.break</t>
   </si>
   <si>
-    <t>Set context.step4</t>
-  </si>
-  <si>
     <t>Set fact.boolValue</t>
   </si>
   <si>
@@ -212,6 +210,75 @@
   </si>
   <si>
     <t>Set result.step1</t>
+  </si>
+  <si>
+    <t>In fact.intValue</t>
+  </si>
+  <si>
+    <t>Out fact.intValue</t>
+  </si>
+  <si>
+    <t>In int</t>
+  </si>
+  <si>
+    <t>1, 3,   5</t>
+  </si>
+  <si>
+    <t>2, 4</t>
+  </si>
+  <si>
+    <t>In str</t>
+  </si>
+  <si>
+    <t>Out int</t>
+  </si>
+  <si>
+    <t>Set context.step3int_in</t>
+  </si>
+  <si>
+    <t>Set context.step3int_out</t>
+  </si>
+  <si>
+    <t>In fact.strValue</t>
+  </si>
+  <si>
+    <t>Out fact.strValue</t>
+  </si>
+  <si>
+    <t>Out str</t>
+  </si>
+  <si>
+    <t>"a", "string with spaces", "b"</t>
+  </si>
+  <si>
+    <t>"c", "d"</t>
+  </si>
+  <si>
+    <t>Set context.step3str_in</t>
+  </si>
+  <si>
+    <t>Set context.step3str_out</t>
+  </si>
+  <si>
+    <t>Set context.step5</t>
+  </si>
+  <si>
+    <t>7, 9</t>
+  </si>
+  <si>
+    <t>"e"</t>
+  </si>
+  <si>
+    <t>Set context.step3last_in</t>
+  </si>
+  <si>
+    <t>Set context.step3last_out</t>
+  </si>
+  <si>
+    <t>Last In</t>
+  </si>
+  <si>
+    <t>Last Out</t>
   </si>
 </sst>
 </file>
@@ -709,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D85D4E-B609-BA4D-A7F3-29129ADE1C24}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -735,48 +802,48 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="H1" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -791,7 +858,7 @@
         <v>44927</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
@@ -828,7 +895,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -853,7 +920,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -933,7 +1000,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -957,7 +1024,7 @@
         <v>35</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>36</v>
@@ -966,7 +1033,7 @@
         <v>36</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1032,11 +1099,145 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F847825A-CCBA-5E4C-BBFD-25B0F218E9E0}">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F02A80BA-6F4C-824B-A578-DF6E4A06F5CC}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1097,12 +1298,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB756B9-053B-3A49-ADCA-1E4932B679E4}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" activeCellId="1" sqref="D11 H23"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1115,7 +1316,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat: add new conditions type, type not, if not and ability to throw errors
</commit_message>
<xml_diff>
--- a/test/assets/rules.xlsx
+++ b/test/assets/rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vlad/Workspace/FireBlink/rulex/test/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098A4FB9-3376-734C-BA62-3FC6F5139BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE6CF3F-E556-714C-A9F3-1D0D5DF350C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6160" yWindow="1240" windowWidth="27240" windowHeight="16440" activeTab="4" xr2:uid="{0B955657-EF69-9248-BFB1-36373A7557EB}"/>
+    <workbookView xWindow="5380" yWindow="2680" windowWidth="27240" windowHeight="16440" activeTab="6" xr2:uid="{0B955657-EF69-9248-BFB1-36373A7557EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Context" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="Step 1 - Condition + Action" sheetId="2" r:id="rId3"/>
     <sheet name="Step 2 - If + Set" sheetId="3" r:id="rId4"/>
     <sheet name="Step 3 - In + Out" sheetId="7" r:id="rId5"/>
-    <sheet name="Step 4 - Break" sheetId="4" r:id="rId6"/>
-    <sheet name="Step 5 - Void" sheetId="5" r:id="rId7"/>
+    <sheet name="Step 4 - Type" sheetId="8" r:id="rId6"/>
+    <sheet name="Step 5 - Break" sheetId="4" r:id="rId7"/>
+    <sheet name="Step 6 - Void" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="96">
   <si>
     <t>Name</t>
   </si>
@@ -260,9 +261,6 @@
     <t>Set context.step3str_out</t>
   </si>
   <si>
-    <t>Set context.step5</t>
-  </si>
-  <si>
     <t>7, 9</t>
   </si>
   <si>
@@ -279,6 +277,60 @@
   </si>
   <si>
     <t>Last Out</t>
+  </si>
+  <si>
+    <t>If not fact.boolValue</t>
+  </si>
+  <si>
+    <t>Not</t>
+  </si>
+  <si>
+    <t>Set context.step2IfNotValue</t>
+  </si>
+  <si>
+    <t>If fact.error</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>fact.error couldn't be true</t>
+  </si>
+  <si>
+    <t>Set context.step6</t>
+  </si>
+  <si>
+    <t>Type fact.boolValue</t>
+  </si>
+  <si>
+    <t>Type not fact.boolValue</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Set context.step4</t>
+  </si>
+  <si>
+    <t>Type fact.strValue</t>
+  </si>
+  <si>
+    <t>Type fact.dateValue</t>
+  </si>
+  <si>
+    <t>Set context.step4blank</t>
+  </si>
+  <si>
+    <t>If not context.initDateValue</t>
+  </si>
+  <si>
+    <t>ERROR E-Test</t>
   </si>
 </sst>
 </file>
@@ -895,7 +947,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -997,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D441B4-1056-A04E-8DBE-9BFDDA9B96D4}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1009,11 +1061,13 @@
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1026,17 +1080,26 @@
       <c r="D1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J1" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -1049,14 +1112,14 @@
       <c r="D2" s="1">
         <v>44774</v>
       </c>
-      <c r="E2" s="3">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
         <v>44562</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1069,14 +1132,14 @@
       <c r="D3" s="1">
         <v>44774</v>
       </c>
-      <c r="E3" s="3">
+      <c r="G3" s="3">
         <v>2</v>
       </c>
-      <c r="G3" s="1">
+      <c r="I3" s="1">
         <v>44563</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1086,11 +1149,25 @@
       <c r="D4" s="1">
         <v>44774</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>3</v>
       </c>
-      <c r="G4" s="1">
+      <c r="I4" s="1">
         <v>44564</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>44775</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1102,7 +1179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F847825A-CCBA-5E4C-BBFD-25B0F218E9E0}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1149,10 +1226,10 @@
         <v>71</v>
       </c>
       <c r="J1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1201,13 +1278,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
         <v>73</v>
-      </c>
-      <c r="D6" t="s">
-        <v>74</v>
       </c>
       <c r="J6" t="b">
         <v>1</v>
@@ -1215,7 +1292,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -1233,63 +1310,166 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F02A80BA-6F4C-824B-A578-DF6E4A06F5CC}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576BE797-0106-E146-9B7B-C01119287933}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="D3" s="1"/>
+      <c r="G3" s="3"/>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F02A80BA-6F4C-824B-A578-DF6E4A06F5CC}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="C3" t="b">
+      <c r="D3" t="b">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
       <c r="E4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1298,12 +1478,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB756B9-053B-3A49-ADCA-1E4932B679E4}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1316,7 +1496,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
test: improve test coverage
</commit_message>
<xml_diff>
--- a/test/assets/rules.xlsx
+++ b/test/assets/rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vlad/Workspace/FireBlink/rulex/test/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE6CF3F-E556-714C-A9F3-1D0D5DF350C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BC3FD4-9717-6648-95C8-E600D6ED7E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5380" yWindow="2680" windowWidth="27240" windowHeight="16440" activeTab="6" xr2:uid="{0B955657-EF69-9248-BFB1-36373A7557EB}"/>
+    <workbookView xWindow="5380" yWindow="2680" windowWidth="27240" windowHeight="16440" activeTab="2" xr2:uid="{0B955657-EF69-9248-BFB1-36373A7557EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Context" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -331,6 +331,21 @@
   </si>
   <si>
     <t>ERROR E-Test</t>
+  </si>
+  <si>
+    <t>context.precondition = true</t>
+  </si>
+  <si>
+    <t>Dependency: Result</t>
+  </si>
+  <si>
+    <t>Dependency: Precondition</t>
+  </si>
+  <si>
+    <t>context.precondition</t>
+  </si>
+  <si>
+    <t>context.dependency = true</t>
   </si>
 </sst>
 </file>
@@ -944,15 +959,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA23193F-2081-EF4F-B2C7-982DC8DDF8B9}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
@@ -1040,6 +1055,28 @@
       </c>
       <c r="E6">
         <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1399,7 +1436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F02A80BA-6F4C-824B-A578-DF6E4A06F5CC}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>

</xml_diff>